<commit_message>
doc: alteração dos caminhos realtivos para inserção de arquivos
</commit_message>
<xml_diff>
--- a/assets/problema_fund_dois.xlsx
+++ b/assets/problema_fund_dois.xlsx
@@ -1,26 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epili\Desktop\Testes_IC\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C53A4B0-E3AB-4D58-918D-6E1A8BA3BF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-20160" yWindow="2100" windowWidth="15375" windowHeight="8325" xr2:uid="{ADCDDA0C-E062-4B6F-9AB4-E6D0893A5054}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -87,7 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,21 +115,21 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
+        <fgColor rgb="FFfff2cc"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE2F0D9"/>
+        <fgColor rgb="FFe2f0d9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFffffff"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -149,87 +139,103 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+  <cellXfs count="17">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -256,116 +262,82 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -377,156 +349,197 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA446BA5-B797-4866-B290-BA68497F7746}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +570,7 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
@@ -576,7 +589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -593,10 +606,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="11">
-        <v>2.9</v>
+        <v>6.9</v>
       </c>
       <c r="G2" s="11">
-        <v>25.254999999999999</v>
+        <v>25.255</v>
       </c>
       <c r="H2" s="12">
         <v>485.9</v>
@@ -605,7 +618,7 @@
         <v>-0.3</v>
       </c>
       <c r="J2" s="12">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="K2" s="12">
         <v>511.6</v>
@@ -626,7 +639,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
@@ -643,7 +656,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="11">
-        <v>7.9850000000000003</v>
+        <v>7.985</v>
       </c>
       <c r="G3" s="11">
         <v>25.105</v>
@@ -655,13 +668,13 @@
         <v>-1</v>
       </c>
       <c r="J3" s="12">
-        <v>9.1999999999999993</v>
+        <v>9.2</v>
       </c>
       <c r="K3" s="12">
         <v>912.1</v>
       </c>
       <c r="L3" s="12">
-        <v>-65.400000000000006</v>
+        <v>-65.4</v>
       </c>
       <c r="M3" s="12">
         <v>0.1</v>
@@ -677,6 +690,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>